<commit_message>
Updated the product backlog
</commit_message>
<xml_diff>
--- a/Backlogs/Product Backlog.xlsx
+++ b/Backlogs/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CSE 327\Project\Backlogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA09FCA-36B4-4DB2-8808-BD9B9407F95A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1179A8-E42B-4963-85EE-AF7EB8C6BA2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{2B8502BF-EC5A-45C2-BE97-16823EFBCC28}"/>
   </bookViews>
@@ -543,7 +543,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +631,7 @@
         <v>34</v>
       </c>
       <c r="F4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Sprint Backlogs and updated product backlog
</commit_message>
<xml_diff>
--- a/Backlogs/Product Backlog.xlsx
+++ b/Backlogs/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CSE 327\Project\Backlogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1179A8-E42B-4963-85EE-AF7EB8C6BA2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBAB58F-DD59-45EC-8E8E-AC070E13D06D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{2B8502BF-EC5A-45C2-BE97-16823EFBCC28}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -72,9 +72,6 @@
     <t>I can sell products to my customers using it without any sort of error in calculation</t>
   </si>
   <si>
-    <t>A sales report option</t>
-  </si>
-  <si>
     <t>I can check and track all the sale details</t>
   </si>
   <si>
@@ -142,6 +139,12 @@
   </si>
   <si>
     <t>Not Started</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Have a sales report option</t>
   </si>
 </sst>
 </file>
@@ -177,15 +180,39 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -208,11 +235,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -221,6 +259,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -540,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E22E15-25BC-4AC9-9106-B9BACA289F7E}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,21 +604,22 @@
     <col min="4" max="4" width="77.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,7 +642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -599,22 +650,22 @@
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -628,16 +679,16 @@
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" s="3">
         <v>2</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -651,16 +702,16 @@
         <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="3">
         <v>2</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -668,22 +719,22 @@
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" s="3">
-        <v>2</v>
-      </c>
-      <c r="G6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -691,22 +742,23 @@
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" s="3">
-        <v>2</v>
-      </c>
-      <c r="G7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -714,22 +766,22 @@
         <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="3">
-        <v>3</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -737,22 +789,22 @@
         <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="E9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" s="3">
-        <v>3</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -760,22 +812,22 @@
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" s="3">
-        <v>3</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -783,22 +835,22 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" s="3">
-        <v>4</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -806,22 +858,22 @@
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="E12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" s="3">
-        <v>4</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -829,22 +881,22 @@
         <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" s="3">
-        <v>4</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -852,19 +904,19 @@
         <v>9</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="E14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F14" s="3">
-        <v>4</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>38</v>
+        <v>5</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>